<commit_message>
new water budget for code v9823 Apr 22 2015
</commit_message>
<xml_diff>
--- a/Willamette_water_budget_.xlsx
+++ b/Willamette_water_budget_.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Willamette_water_budget_" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="33">
   <si>
     <t>Scenario</t>
   </si>
@@ -104,6 +104,15 @@
   </si>
   <si>
     <t>2070 - 2100 Extreme sc</t>
+  </si>
+  <si>
+    <t>EXTREME</t>
+  </si>
+  <si>
+    <t>HIGH CLIM</t>
+  </si>
+  <si>
+    <t>REFERENCE</t>
   </si>
 </sst>
 </file>
@@ -900,11 +909,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="49684864"/>
-        <c:axId val="49686784"/>
+        <c:axId val="159054848"/>
+        <c:axId val="134222592"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="49684864"/>
+        <c:axId val="159054848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -913,7 +922,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49686784"/>
+        <c:crossAx val="134222592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -921,7 +930,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="49686784"/>
+        <c:axId val="134222592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -931,7 +940,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49684864"/>
+        <c:crossAx val="159054848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -957,16 +966,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>228599</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>42862</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>380999</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>123824</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>276224</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1275,15 +1284,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AZ14"/>
+  <dimension ref="A1:AZ22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T19" sqref="T19"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="Z27" sqref="Z27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:52" x14ac:dyDescent="0.25">
@@ -1326,6 +1337,15 @@
       <c r="M1" t="s">
         <v>12</v>
       </c>
+      <c r="P1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="2" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -3379,6 +3399,94 @@
       </c>
       <c r="AZ14">
         <v>6.0467526169499998E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="11:51" x14ac:dyDescent="0.25">
+      <c r="K18">
+        <f>SUM(K4:K9)</f>
+        <v>90.831597109300006</v>
+      </c>
+      <c r="X18">
+        <f>SUM(X4:X9)</f>
+        <v>106.76311385339999</v>
+      </c>
+      <c r="AK18">
+        <f>SUM(AK4:AK9)</f>
+        <v>97.392651081100013</v>
+      </c>
+      <c r="AX18">
+        <f>SUM(AX4:AX9)</f>
+        <v>94.988924375499991</v>
+      </c>
+    </row>
+    <row r="20" spans="11:51" x14ac:dyDescent="0.25">
+      <c r="K20">
+        <f>0.1*K18*240000</f>
+        <v>2179958.3306232002</v>
+      </c>
+      <c r="X20">
+        <f>0.1*X18*240000</f>
+        <v>2562314.7324815998</v>
+      </c>
+      <c r="AK20">
+        <f>0.1*AK18*240000</f>
+        <v>2337423.6259464007</v>
+      </c>
+      <c r="AX20">
+        <f>0.1*AX18*240000</f>
+        <v>2279734.1850119997</v>
+      </c>
+    </row>
+    <row r="21" spans="11:51" x14ac:dyDescent="0.25">
+      <c r="K21">
+        <f>K20*326000</f>
+        <v>710666415783.16321</v>
+      </c>
+      <c r="L21" s="1">
+        <f>K21/100/365</f>
+        <v>19470312.761182554</v>
+      </c>
+      <c r="X21">
+        <f>X20*326000</f>
+        <v>835314602789.00159</v>
+      </c>
+      <c r="Y21" s="1">
+        <f>X21/100/365</f>
+        <v>22885331.583260316</v>
+      </c>
+      <c r="AK21">
+        <f>AK20*326000</f>
+        <v>762000102058.52661</v>
+      </c>
+      <c r="AL21" s="1">
+        <f>AK21/100/365</f>
+        <v>20876715.12489114</v>
+      </c>
+      <c r="AX21">
+        <f>AX20*326000</f>
+        <v>743193344313.91187</v>
+      </c>
+      <c r="AY21" s="1">
+        <f>AX21/100/365</f>
+        <v>20361461.488052379</v>
+      </c>
+    </row>
+    <row r="22" spans="11:51" x14ac:dyDescent="0.25">
+      <c r="K22" s="1">
+        <f>K21*0.005</f>
+        <v>3553332078.9158163</v>
+      </c>
+      <c r="X22" s="1">
+        <f>X21*0.005</f>
+        <v>4176573013.9450078</v>
+      </c>
+      <c r="AK22" s="1">
+        <f>AK21*0.005</f>
+        <v>3810000510.2926331</v>
+      </c>
+      <c r="AX22" s="1">
+        <f>AX21*0.005</f>
+        <v>3715966721.5695596</v>
       </c>
     </row>
   </sheetData>

</xml_diff>